<commit_message>
removendo variaveis não utilizadas
</commit_message>
<xml_diff>
--- a/lista de termos.xlsx
+++ b/lista de termos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cd8d193c451d04b/Documentos/VsCode Projects/extracao-termo-marinha-main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cd8d193c451d04b/Documentos/VsCode Projects/termo-afrmm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_AD4D361C20488DEA4E38A0FB84D97FD65BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FB0CE80-845B-4FA4-97F8-794B666255BA}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_AD4D361C20488DEA4E38A0FB84D97FD65BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3021EEE-C828-4236-9354-9CB024C918F6}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>Sua Referencia</t>
   </si>
@@ -368,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +404,38 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>